<commit_message>
updated blanks in Tri_ela 2017 count
</commit_message>
<xml_diff>
--- a/00_Data/Master_files/count_data_MASTER.xlsx
+++ b/00_Data/Master_files/count_data_MASTER.xlsx
@@ -17,7 +17,7 @@
     <sheet name="count_2018" sheetId="2" r:id="rId3"/>
     <sheet name="count_2019" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2769,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR49"/>
   <sheetViews>
-    <sheetView topLeftCell="DB1" workbookViewId="0">
-      <selection activeCell="DE20" sqref="DE20"/>
+    <sheetView topLeftCell="CQ19" workbookViewId="0">
+      <selection activeCell="CX27" sqref="CX27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -20821,15 +20821,16 @@
   <dimension ref="A1:DR49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="DD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="CX1" sqref="CX1:CX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="102" max="102" width="10.6640625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:122" x14ac:dyDescent="0.35">
@@ -21136,7 +21137,7 @@
       <c r="CW1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CX1" s="11" t="s">
         <v>101</v>
       </c>
       <c r="CY1" t="s">
@@ -21504,7 +21505,7 @@
       <c r="CW2">
         <v>0</v>
       </c>
-      <c r="CX2">
+      <c r="CX2" s="11">
         <v>1</v>
       </c>
       <c r="CY2">
@@ -21872,7 +21873,7 @@
       <c r="CW3">
         <v>1</v>
       </c>
-      <c r="CX3">
+      <c r="CX3" s="11">
         <v>0</v>
       </c>
       <c r="CY3">
@@ -22240,7 +22241,7 @@
       <c r="CW4">
         <v>0</v>
       </c>
-      <c r="CX4">
+      <c r="CX4" s="11">
         <v>0</v>
       </c>
       <c r="CY4">
@@ -22608,7 +22609,7 @@
       <c r="CW5">
         <v>0</v>
       </c>
-      <c r="CX5">
+      <c r="CX5" s="11">
         <v>4</v>
       </c>
       <c r="CY5">
@@ -22976,7 +22977,7 @@
       <c r="CW6">
         <v>0</v>
       </c>
-      <c r="CX6">
+      <c r="CX6" s="11">
         <v>8</v>
       </c>
       <c r="CY6">
@@ -23344,7 +23345,7 @@
       <c r="CW7">
         <v>0</v>
       </c>
-      <c r="CX7">
+      <c r="CX7" s="11">
         <v>1</v>
       </c>
       <c r="CY7">
@@ -23712,7 +23713,7 @@
       <c r="CW8">
         <v>0</v>
       </c>
-      <c r="CX8">
+      <c r="CX8" s="11">
         <v>0</v>
       </c>
       <c r="CY8">
@@ -24080,7 +24081,7 @@
       <c r="CW9">
         <v>0</v>
       </c>
-      <c r="CX9">
+      <c r="CX9" s="11">
         <v>0</v>
       </c>
       <c r="CY9">
@@ -24448,7 +24449,7 @@
       <c r="CW10">
         <v>0</v>
       </c>
-      <c r="CX10">
+      <c r="CX10" s="11">
         <v>3</v>
       </c>
       <c r="CY10">
@@ -24816,7 +24817,7 @@
       <c r="CW11">
         <v>1</v>
       </c>
-      <c r="CX11">
+      <c r="CX11" s="11">
         <v>3</v>
       </c>
       <c r="CY11">
@@ -25184,7 +25185,7 @@
       <c r="CW12">
         <v>0</v>
       </c>
-      <c r="CX12">
+      <c r="CX12" s="11">
         <v>6</v>
       </c>
       <c r="CY12">
@@ -25552,7 +25553,7 @@
       <c r="CW13">
         <v>0</v>
       </c>
-      <c r="CX13">
+      <c r="CX13" s="11">
         <v>20</v>
       </c>
       <c r="CY13">
@@ -25920,7 +25921,7 @@
       <c r="CW14">
         <v>0</v>
       </c>
-      <c r="CX14">
+      <c r="CX14" s="11">
         <v>1</v>
       </c>
       <c r="CY14">
@@ -26288,7 +26289,7 @@
       <c r="CW15">
         <v>1</v>
       </c>
-      <c r="CX15">
+      <c r="CX15" s="11">
         <v>1</v>
       </c>
       <c r="CY15">
@@ -26656,7 +26657,7 @@
       <c r="CW16">
         <v>1</v>
       </c>
-      <c r="CX16">
+      <c r="CX16" s="11">
         <v>2</v>
       </c>
       <c r="CY16">
@@ -27024,7 +27025,7 @@
       <c r="CW17">
         <v>0</v>
       </c>
-      <c r="CX17">
+      <c r="CX17" s="11">
         <v>7</v>
       </c>
       <c r="CY17">
@@ -27392,7 +27393,7 @@
       <c r="CW18">
         <v>0</v>
       </c>
-      <c r="CX18">
+      <c r="CX18" s="11">
         <v>11</v>
       </c>
       <c r="CY18">
@@ -27760,7 +27761,7 @@
       <c r="CW19">
         <v>0</v>
       </c>
-      <c r="CX19">
+      <c r="CX19" s="11">
         <v>1</v>
       </c>
       <c r="CY19">
@@ -28128,7 +28129,7 @@
       <c r="CW20">
         <v>0</v>
       </c>
-      <c r="CX20">
+      <c r="CX20" s="11">
         <v>0</v>
       </c>
       <c r="CY20">
@@ -28496,7 +28497,7 @@
       <c r="CW21">
         <v>0</v>
       </c>
-      <c r="CX21">
+      <c r="CX21" s="11">
         <v>2</v>
       </c>
       <c r="CY21">
@@ -28864,7 +28865,7 @@
       <c r="CW22">
         <v>0</v>
       </c>
-      <c r="CX22">
+      <c r="CX22" s="11">
         <v>2</v>
       </c>
       <c r="CY22">
@@ -29232,7 +29233,7 @@
       <c r="CW23">
         <v>0</v>
       </c>
-      <c r="CX23">
+      <c r="CX23" s="11">
         <v>14</v>
       </c>
       <c r="CY23">
@@ -29600,7 +29601,7 @@
       <c r="CW24">
         <v>0</v>
       </c>
-      <c r="CX24">
+      <c r="CX24" s="11">
         <v>13</v>
       </c>
       <c r="CY24">
@@ -29968,7 +29969,7 @@
       <c r="CW25">
         <v>0</v>
       </c>
-      <c r="CX25">
+      <c r="CX25" s="11">
         <v>5</v>
       </c>
       <c r="CY25">
@@ -30336,7 +30337,7 @@
       <c r="CW26">
         <v>0</v>
       </c>
-      <c r="CX26">
+      <c r="CX26" s="11">
         <v>13</v>
       </c>
       <c r="CY26">
@@ -30704,7 +30705,7 @@
       <c r="CW27">
         <v>0</v>
       </c>
-      <c r="CX27">
+      <c r="CX27" s="11">
         <v>3</v>
       </c>
       <c r="CY27">
@@ -31072,7 +31073,7 @@
       <c r="CW28">
         <v>0</v>
       </c>
-      <c r="CX28">
+      <c r="CX28" s="11">
         <v>15</v>
       </c>
       <c r="CY28">
@@ -31440,7 +31441,7 @@
       <c r="CW29">
         <v>0</v>
       </c>
-      <c r="CX29">
+      <c r="CX29" s="11">
         <v>3</v>
       </c>
       <c r="CY29">
@@ -31808,7 +31809,7 @@
       <c r="CW30">
         <v>0</v>
       </c>
-      <c r="CX30">
+      <c r="CX30" s="11">
         <v>4</v>
       </c>
       <c r="CY30">
@@ -32176,7 +32177,7 @@
       <c r="CW31">
         <v>0</v>
       </c>
-      <c r="CX31">
+      <c r="CX31" s="11">
         <v>7</v>
       </c>
       <c r="CY31">
@@ -32544,7 +32545,7 @@
       <c r="CW32">
         <v>1</v>
       </c>
-      <c r="CX32">
+      <c r="CX32" s="11">
         <v>0</v>
       </c>
       <c r="CY32">
@@ -32912,7 +32913,7 @@
       <c r="CW33">
         <v>0</v>
       </c>
-      <c r="CX33">
+      <c r="CX33" s="11">
         <v>6</v>
       </c>
       <c r="CY33">
@@ -33280,7 +33281,7 @@
       <c r="CW34">
         <v>0</v>
       </c>
-      <c r="CX34">
+      <c r="CX34" s="11">
         <v>9</v>
       </c>
       <c r="CY34">
@@ -33648,7 +33649,7 @@
       <c r="CW35">
         <v>0</v>
       </c>
-      <c r="CX35">
+      <c r="CX35" s="11">
         <v>10</v>
       </c>
       <c r="CY35">
@@ -34016,7 +34017,7 @@
       <c r="CW36">
         <v>0</v>
       </c>
-      <c r="CX36">
+      <c r="CX36" s="11">
         <v>3</v>
       </c>
       <c r="CY36">
@@ -34384,7 +34385,7 @@
       <c r="CW37">
         <v>0</v>
       </c>
-      <c r="CX37">
+      <c r="CX37" s="11">
         <v>5</v>
       </c>
       <c r="CY37">
@@ -34752,7 +34753,7 @@
       <c r="CW38">
         <v>0</v>
       </c>
-      <c r="CX38">
+      <c r="CX38" s="11">
         <v>0</v>
       </c>
       <c r="CY38">
@@ -35120,7 +35121,7 @@
       <c r="CW39">
         <v>0</v>
       </c>
-      <c r="CX39">
+      <c r="CX39" s="11">
         <v>0</v>
       </c>
       <c r="CY39">
@@ -35488,7 +35489,7 @@
       <c r="CW40">
         <v>0</v>
       </c>
-      <c r="CX40">
+      <c r="CX40" s="11">
         <v>2</v>
       </c>
       <c r="CY40">
@@ -35856,7 +35857,7 @@
       <c r="CW41">
         <v>0</v>
       </c>
-      <c r="CX41">
+      <c r="CX41" s="11">
         <v>0</v>
       </c>
       <c r="CY41">
@@ -36224,7 +36225,7 @@
       <c r="CW42">
         <v>0</v>
       </c>
-      <c r="CX42">
+      <c r="CX42" s="11">
         <v>0</v>
       </c>
       <c r="CY42">
@@ -36592,7 +36593,7 @@
       <c r="CW43">
         <v>0</v>
       </c>
-      <c r="CX43">
+      <c r="CX43" s="11">
         <v>0</v>
       </c>
       <c r="CY43">
@@ -36960,7 +36961,7 @@
       <c r="CW44">
         <v>0</v>
       </c>
-      <c r="CX44">
+      <c r="CX44" s="11">
         <v>0</v>
       </c>
       <c r="CY44">
@@ -37328,7 +37329,7 @@
       <c r="CW45">
         <v>0</v>
       </c>
-      <c r="CX45">
+      <c r="CX45" s="11">
         <v>0</v>
       </c>
       <c r="CY45">
@@ -37696,7 +37697,7 @@
       <c r="CW46">
         <v>0</v>
       </c>
-      <c r="CX46">
+      <c r="CX46" s="11">
         <v>0</v>
       </c>
       <c r="CY46">
@@ -38064,7 +38065,7 @@
       <c r="CW47">
         <v>0</v>
       </c>
-      <c r="CX47">
+      <c r="CX47" s="11">
         <v>2</v>
       </c>
       <c r="CY47">
@@ -38432,7 +38433,7 @@
       <c r="CW48">
         <v>0</v>
       </c>
-      <c r="CX48">
+      <c r="CX48" s="11">
         <v>0</v>
       </c>
       <c r="CY48">
@@ -38800,7 +38801,7 @@
       <c r="CW49">
         <v>0</v>
       </c>
-      <c r="CX49">
+      <c r="CX49" s="11">
         <v>0</v>
       </c>
       <c r="CY49">
@@ -38873,13 +38874,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
-      <selection activeCell="DI13" sqref="DI13"/>
+    <sheetView tabSelected="1" topLeftCell="CQ28" workbookViewId="0">
+      <selection activeCell="CX1" sqref="CX1:CX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="102" max="102" width="10.6640625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:122" x14ac:dyDescent="0.35">
@@ -39186,7 +39188,7 @@
       <c r="CW1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CX1" s="11" t="s">
         <v>101</v>
       </c>
       <c r="CY1" t="s">
@@ -39554,7 +39556,7 @@
       <c r="CW2">
         <v>0</v>
       </c>
-      <c r="CX2">
+      <c r="CX2" s="11">
         <v>1</v>
       </c>
       <c r="CY2">
@@ -39922,7 +39924,7 @@
       <c r="CW3">
         <v>0</v>
       </c>
-      <c r="CX3">
+      <c r="CX3" s="11">
         <v>0</v>
       </c>
       <c r="CY3">
@@ -40290,7 +40292,7 @@
       <c r="CW4">
         <v>0</v>
       </c>
-      <c r="CX4">
+      <c r="CX4" s="11">
         <v>0</v>
       </c>
       <c r="CY4">
@@ -40658,7 +40660,7 @@
       <c r="CW5">
         <v>0</v>
       </c>
-      <c r="CX5">
+      <c r="CX5" s="11">
         <v>4</v>
       </c>
       <c r="CY5">
@@ -41026,7 +41028,7 @@
       <c r="CW6">
         <v>0</v>
       </c>
-      <c r="CX6">
+      <c r="CX6" s="11">
         <v>13</v>
       </c>
       <c r="CY6">
@@ -41394,7 +41396,7 @@
       <c r="CW7">
         <v>0</v>
       </c>
-      <c r="CX7">
+      <c r="CX7" s="11">
         <v>1</v>
       </c>
       <c r="CY7">
@@ -41762,7 +41764,7 @@
       <c r="CW8">
         <v>0</v>
       </c>
-      <c r="CX8">
+      <c r="CX8" s="11">
         <v>0</v>
       </c>
       <c r="CY8">
@@ -42130,7 +42132,7 @@
       <c r="CW9">
         <v>0</v>
       </c>
-      <c r="CX9">
+      <c r="CX9" s="11">
         <v>0</v>
       </c>
       <c r="CY9">
@@ -42498,7 +42500,7 @@
       <c r="CW10">
         <v>0</v>
       </c>
-      <c r="CX10">
+      <c r="CX10" s="11">
         <v>0</v>
       </c>
       <c r="CY10">
@@ -42866,7 +42868,7 @@
       <c r="CW11">
         <v>1</v>
       </c>
-      <c r="CX11">
+      <c r="CX11" s="11">
         <v>1</v>
       </c>
       <c r="CY11">
@@ -43234,7 +43236,7 @@
       <c r="CW12">
         <v>0</v>
       </c>
-      <c r="CX12">
+      <c r="CX12" s="11">
         <v>4</v>
       </c>
       <c r="CY12">
@@ -43602,7 +43604,7 @@
       <c r="CW13">
         <v>0</v>
       </c>
-      <c r="CX13">
+      <c r="CX13" s="11">
         <v>15</v>
       </c>
       <c r="CY13">
@@ -43970,7 +43972,7 @@
       <c r="CW14">
         <v>0</v>
       </c>
-      <c r="CX14">
+      <c r="CX14" s="11">
         <v>0</v>
       </c>
       <c r="CY14">
@@ -44338,7 +44340,7 @@
       <c r="CW15">
         <v>1</v>
       </c>
-      <c r="CX15">
+      <c r="CX15" s="11">
         <v>1</v>
       </c>
       <c r="CY15">
@@ -44706,7 +44708,7 @@
       <c r="CW16">
         <v>0</v>
       </c>
-      <c r="CX16">
+      <c r="CX16" s="11">
         <v>4</v>
       </c>
       <c r="CY16">
@@ -45074,7 +45076,7 @@
       <c r="CW17">
         <v>0</v>
       </c>
-      <c r="CX17">
+      <c r="CX17" s="11">
         <v>8</v>
       </c>
       <c r="CY17">
@@ -45442,7 +45444,7 @@
       <c r="CW18">
         <v>0</v>
       </c>
-      <c r="CX18">
+      <c r="CX18" s="11">
         <v>18</v>
       </c>
       <c r="CY18">
@@ -45810,7 +45812,7 @@
       <c r="CW19">
         <v>0</v>
       </c>
-      <c r="CX19">
+      <c r="CX19" s="11">
         <v>1</v>
       </c>
       <c r="CY19">
@@ -46178,7 +46180,7 @@
       <c r="CW20">
         <v>0</v>
       </c>
-      <c r="CX20">
+      <c r="CX20" s="11">
         <v>0</v>
       </c>
       <c r="CY20">
@@ -46546,7 +46548,7 @@
       <c r="CW21">
         <v>0</v>
       </c>
-      <c r="CX21">
+      <c r="CX21" s="11">
         <v>1</v>
       </c>
       <c r="CY21">
@@ -46914,7 +46916,7 @@
       <c r="CW22">
         <v>0</v>
       </c>
-      <c r="CX22">
+      <c r="CX22" s="11">
         <v>3</v>
       </c>
       <c r="CY22">
@@ -47282,7 +47284,7 @@
       <c r="CW23">
         <v>0</v>
       </c>
-      <c r="CX23">
+      <c r="CX23" s="11">
         <v>11</v>
       </c>
       <c r="CY23">
@@ -47650,7 +47652,7 @@
       <c r="CW24">
         <v>0</v>
       </c>
-      <c r="CX24">
+      <c r="CX24" s="11">
         <v>14</v>
       </c>
       <c r="CY24">
@@ -48018,7 +48020,7 @@
       <c r="CW25">
         <v>0</v>
       </c>
-      <c r="CX25">
+      <c r="CX25" s="11">
         <v>11</v>
       </c>
       <c r="CY25">
@@ -48386,7 +48388,7 @@
       <c r="CW26">
         <v>0</v>
       </c>
-      <c r="CX26">
+      <c r="CX26" s="11">
         <v>12</v>
       </c>
       <c r="CY26">
@@ -48754,7 +48756,7 @@
       <c r="CW27">
         <v>0</v>
       </c>
-      <c r="CX27">
+      <c r="CX27" s="11">
         <v>0</v>
       </c>
       <c r="CY27">
@@ -49122,7 +49124,7 @@
       <c r="CW28">
         <v>0</v>
       </c>
-      <c r="CX28">
+      <c r="CX28" s="11">
         <v>8</v>
       </c>
       <c r="CY28">
@@ -49490,7 +49492,7 @@
       <c r="CW29">
         <v>0</v>
       </c>
-      <c r="CX29">
+      <c r="CX29" s="11">
         <v>3</v>
       </c>
       <c r="CY29">
@@ -49858,7 +49860,7 @@
       <c r="CW30">
         <v>0</v>
       </c>
-      <c r="CX30">
+      <c r="CX30" s="11">
         <v>3</v>
       </c>
       <c r="CY30">
@@ -50226,7 +50228,7 @@
       <c r="CW31">
         <v>0</v>
       </c>
-      <c r="CX31">
+      <c r="CX31" s="11">
         <v>6</v>
       </c>
       <c r="CY31">
@@ -50594,7 +50596,7 @@
       <c r="CW32">
         <v>0</v>
       </c>
-      <c r="CX32">
+      <c r="CX32" s="11">
         <v>0</v>
       </c>
       <c r="CY32">
@@ -50962,7 +50964,7 @@
       <c r="CW33">
         <v>0</v>
       </c>
-      <c r="CX33">
+      <c r="CX33" s="11">
         <v>0</v>
       </c>
       <c r="CY33">
@@ -51330,7 +51332,7 @@
       <c r="CW34">
         <v>0</v>
       </c>
-      <c r="CX34">
+      <c r="CX34" s="11">
         <v>2</v>
       </c>
       <c r="CY34">
@@ -51698,7 +51700,7 @@
       <c r="CW35">
         <v>0</v>
       </c>
-      <c r="CX35">
+      <c r="CX35" s="11">
         <v>6</v>
       </c>
       <c r="CY35">
@@ -52066,7 +52068,7 @@
       <c r="CW36">
         <v>0</v>
       </c>
-      <c r="CX36">
+      <c r="CX36" s="11">
         <v>2</v>
       </c>
       <c r="CY36">
@@ -52434,7 +52436,7 @@
       <c r="CW37">
         <v>0</v>
       </c>
-      <c r="CX37">
+      <c r="CX37" s="11">
         <v>2</v>
       </c>
       <c r="CY37">
@@ -52802,7 +52804,7 @@
       <c r="CW38">
         <v>0</v>
       </c>
-      <c r="CX38">
+      <c r="CX38" s="11">
         <v>0</v>
       </c>
       <c r="CY38">
@@ -53170,7 +53172,7 @@
       <c r="CW39">
         <v>0</v>
       </c>
-      <c r="CX39">
+      <c r="CX39" s="11">
         <v>0</v>
       </c>
       <c r="CY39">
@@ -53538,7 +53540,7 @@
       <c r="CW40">
         <v>0</v>
       </c>
-      <c r="CX40">
+      <c r="CX40" s="11">
         <v>2</v>
       </c>
       <c r="CY40">
@@ -53906,7 +53908,7 @@
       <c r="CW41">
         <v>0</v>
       </c>
-      <c r="CX41">
+      <c r="CX41" s="11">
         <v>0</v>
       </c>
       <c r="CY41">
@@ -54274,7 +54276,7 @@
       <c r="CW42">
         <v>0</v>
       </c>
-      <c r="CX42">
+      <c r="CX42" s="11">
         <v>0</v>
       </c>
       <c r="CY42">
@@ -54642,7 +54644,7 @@
       <c r="CW43">
         <v>0</v>
       </c>
-      <c r="CX43">
+      <c r="CX43" s="11">
         <v>0</v>
       </c>
       <c r="CY43">
@@ -55010,7 +55012,7 @@
       <c r="CW44">
         <v>0</v>
       </c>
-      <c r="CX44">
+      <c r="CX44" s="11">
         <v>0</v>
       </c>
       <c r="CY44">
@@ -55378,7 +55380,7 @@
       <c r="CW45">
         <v>0</v>
       </c>
-      <c r="CX45">
+      <c r="CX45" s="11">
         <v>0</v>
       </c>
       <c r="CY45">
@@ -55746,7 +55748,7 @@
       <c r="CW46">
         <v>0</v>
       </c>
-      <c r="CX46">
+      <c r="CX46" s="11">
         <v>0</v>
       </c>
       <c r="CY46">
@@ -56114,7 +56116,7 @@
       <c r="CW47">
         <v>0</v>
       </c>
-      <c r="CX47">
+      <c r="CX47" s="11">
         <v>2</v>
       </c>
       <c r="CY47">
@@ -56482,7 +56484,7 @@
       <c r="CW48">
         <v>0</v>
       </c>
-      <c r="CX48">
+      <c r="CX48" s="11">
         <v>1</v>
       </c>
       <c r="CY48">
@@ -56850,7 +56852,7 @@
       <c r="CW49">
         <v>0</v>
       </c>
-      <c r="CX49">
+      <c r="CX49" s="11">
         <v>0</v>
       </c>
       <c r="CY49">

</xml_diff>